<commit_message>
cleanup updated - new cleaned sample created - columns from excel now excluded from dataset
</commit_message>
<xml_diff>
--- a/Description of Dataset.xlsx
+++ b/Description of Dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhnw365.sharepoint.com/teams/O365_G_Data_Science_AS20-GroupA2/Freigegebene Dokumente/Group A2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\switchdrive\Data Science\Assignment\Lending-Club-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="402" documentId="8_{EF867EF5-4F87-4AE9-B538-30831425B432}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{54AB6F3D-1CF1-40F0-905C-7B59030B48B5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1D84D2-F3CD-4396-AE05-C1200454B448}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-285" windowWidth="29040" windowHeight="17640" xr2:uid="{3D298F21-2F40-4ACD-AA0D-9D5528E80E5D}"/>
+    <workbookView minimized="1" xWindow="-24900" yWindow="3900" windowWidth="21600" windowHeight="12600" xr2:uid="{3D298F21-2F40-4ACD-AA0D-9D5528E80E5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Classification" sheetId="1" r:id="rId1"/>
@@ -1219,7 +1219,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1278,14 +1278,6 @@
     </font>
     <font>
       <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1489,9 +1481,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1538,9 +1530,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1972,10 +1963,10 @@
   <dimension ref="A1:H78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3136,7 +3127,7 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="40" t="s">
+      <c r="A54" s="35" t="s">
         <v>131</v>
       </c>
       <c r="B54" s="3" t="s">
@@ -3182,7 +3173,7 @@
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="41" t="s">
+      <c r="A56" s="40" t="s">
         <v>138</v>
       </c>
       <c r="B56" s="3" t="s">
@@ -3206,7 +3197,7 @@
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="41" t="s">
+      <c r="A57" s="40" t="s">
         <v>142</v>
       </c>
       <c r="B57" s="3" t="s">
@@ -3660,7 +3651,7 @@
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="42" t="s">
+      <c r="A78" s="41" t="s">
         <v>380</v>
       </c>
     </row>
@@ -5350,18 +5341,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5497,14 +5488,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB4C82CF-0596-4755-BB63-87CF708610A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{688AF489-0CED-4555-A0AC-B0C0E95288CD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -5516,6 +5499,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB4C82CF-0596-4755-BB63-87CF708610A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>